<commit_message>
[ORI] 17/11/19 - fix the error in the power)state script, and continue the accelerometer script
</commit_message>
<xml_diff>
--- a/cyber_traits_hours.xlsx
+++ b/cyber_traits_hours.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yafit Shneor\Desktop\cyberTraits11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yafit Shneor\GitHub\cyberTraits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C01158-6482-4586-BA19-215571201CB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1771CF-F6EF-455F-8F1D-7EB825585F7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1E004A04-5E3F-4E0A-BD1B-1F5248A47DD5}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="128">
   <si>
     <t>Column1</t>
   </si>
@@ -511,6 +511,12 @@
   </si>
   <si>
     <t xml:space="preserve">יפית - עבודה עם גיט </t>
+  </si>
+  <si>
+    <t>17.11.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">אורי - פתירת הבעיה של POWER STATE וקצת על תאוצה                </t>
   </si>
 </sst>
 </file>
@@ -1098,8 +1104,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A222D9DB-94B1-4D6D-B5C9-B354B9FBBD85}" name="טבלה4" displayName="טבלה4" ref="A1:D21" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16">
-  <autoFilter ref="A1:D21" xr:uid="{A5919AAF-61B8-46D6-B675-8847E2D31601}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A222D9DB-94B1-4D6D-B5C9-B354B9FBBD85}" name="טבלה4" displayName="טבלה4" ref="A1:D22" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16">
+  <autoFilter ref="A1:D22" xr:uid="{A5919AAF-61B8-46D6-B675-8847E2D31601}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{6162BB0C-393B-474E-BF83-430D1C7FD506}" name="תאריך למנ'" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{29CE8E1F-3EE4-46A8-8A75-258713F17C35}" name="מספר שעות" dataDxfId="14"/>
@@ -1641,10 +1647,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC85EBA-B126-46C8-BAEB-25B2C09B38D0}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C26" sqref="C25:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1897,6 +1903,18 @@
         <v>125</v>
       </c>
       <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" s="18">
+        <v>3.5</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
[YAFIT] update code + main and questionaries
</commit_message>
<xml_diff>
--- a/cyber_traits_hours.xlsx
+++ b/cyber_traits_hours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yafit Shneor\GitHub\cyberTraits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1771CF-F6EF-455F-8F1D-7EB825585F7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496CAF8C-234E-4626-9859-381F79EF2F6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1E004A04-5E3F-4E0A-BD1B-1F5248A47DD5}"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8916" activeTab="1" xr2:uid="{1E004A04-5E3F-4E0A-BD1B-1F5248A47DD5}"/>
   </bookViews>
   <sheets>
     <sheet name="data from the beiwe app" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="132">
   <si>
     <t>Column1</t>
   </si>
@@ -517,6 +517,18 @@
   </si>
   <si>
     <t xml:space="preserve">אורי - פתירת הבעיה של POWER STATE וקצת על תאוצה                </t>
+  </si>
+  <si>
+    <t>19.11.19</t>
+  </si>
+  <si>
+    <t>פגישה עם חסיןן המשכת קוד תאוצה- סיימנו מילוי טרלו</t>
+  </si>
+  <si>
+    <t>דיברנו עם יוני על השאלונים, ועדכנו קוד</t>
+  </si>
+  <si>
+    <t>יפית - עדכון בגיט ועדכון השינויים בקוד</t>
   </si>
 </sst>
 </file>
@@ -691,7 +703,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -745,6 +757,9 @@
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
     </xf>
   </cellXfs>
@@ -1104,8 +1119,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A222D9DB-94B1-4D6D-B5C9-B354B9FBBD85}" name="טבלה4" displayName="טבלה4" ref="A1:D22" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16">
-  <autoFilter ref="A1:D22" xr:uid="{A5919AAF-61B8-46D6-B675-8847E2D31601}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A222D9DB-94B1-4D6D-B5C9-B354B9FBBD85}" name="טבלה4" displayName="טבלה4" ref="A1:D25" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16">
+  <autoFilter ref="A1:D25" xr:uid="{A5919AAF-61B8-46D6-B675-8847E2D31601}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{6162BB0C-393B-474E-BF83-430D1C7FD506}" name="תאריך למנ'" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{29CE8E1F-3EE4-46A8-8A75-258713F17C35}" name="מספר שעות" dataDxfId="14"/>
@@ -1647,10 +1662,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC85EBA-B126-46C8-BAEB-25B2C09B38D0}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C26" sqref="C25:C26"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1904,7 +1919,7 @@
       </c>
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>126</v>
       </c>
@@ -1915,6 +1930,40 @@
         <v>127</v>
       </c>
       <c r="D22" s="18"/>
+    </row>
+    <row r="23" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B23" s="18">
+        <v>7</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D23" s="18"/>
+    </row>
+    <row r="24" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="19">
+        <v>43789</v>
+      </c>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="D24" s="18"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="17">
+        <v>21.11</v>
+      </c>
+      <c r="B25" s="18">
+        <v>1</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D25" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>